<commit_message>
First cut at tile colors
</commit_message>
<xml_diff>
--- a/Docs/Tile Types.xlsx
+++ b/Docs/Tile Types.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="106">
   <si>
     <t>Empty Space</t>
   </si>
@@ -334,6 +334,9 @@
   </si>
   <si>
     <t>Water?</t>
+  </si>
+  <si>
+    <t>Secret Door?</t>
   </si>
 </sst>
 </file>
@@ -707,7 +710,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -718,7 +721,7 @@
   <dimension ref="B2:Q207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,6 +1336,9 @@
       <c r="B17" s="1">
         <v>14</v>
       </c>
+      <c r="C17" t="s">
+        <v>105</v>
+      </c>
       <c r="D17" s="1">
         <v>46</v>
       </c>

</xml_diff>